<commit_message>
ticket 170: ajuste en plantilla de OS de CNT
</commit_message>
<xml_diff>
--- a/public/uploads/${ID_SERVICIO} Orden ${ID_SERVICIO_LETRAS} ${EXTREMO_CIU_NOMBRE} ${ID_SERVICIO}.xlsx
+++ b/public/uploads/${ID_SERVICIO} Orden ${ID_SERVICIO_LETRAS} ${EXTREMO_CIU_NOMBRE} ${ID_SERVICIO}.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve"> ${CAPACIDAD_SOLICITADA} MB</t>
   </si>
   <si>
-    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION} $</t>
+    <t xml:space="preserve">${CONCENTRADOR_UBI_DIRECCION}</t>
   </si>
   <si>
     <t xml:space="preserve">${CON_NOMBRES} ${CON_APELLIDOS} </t>
@@ -247,8 +247,8 @@
   </sheetPr>
   <dimension ref="A2:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>